<commit_message>
Updates on Sat Aug 6 16:48:14 2016 -0400
</commit_message>
<xml_diff>
--- a/proposal/dcache/plots/dovecot.xlsx
+++ b/proposal/dcache/plots/dovecot.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiache/Workspace/oscar/dcache-optimization/papers/sosp15/plots/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiache/Workspace/oscar/chiache-thesis/proposal/dcache/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -508,11 +511,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-50"/>
-        <c:axId val="-2089583856"/>
-        <c:axId val="-2117861984"/>
+        <c:axId val="2075752816"/>
+        <c:axId val="2142582544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2089583856"/>
+        <c:axId val="2075752816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -566,7 +569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117861984"/>
+        <c:crossAx val="2142582544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -574,7 +577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117861984"/>
+        <c:axId val="2142582544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350.0"/>
@@ -651,7 +654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089583856"/>
+        <c:crossAx val="2075752816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -769,9 +772,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.189320948468221"/>
+          <c:x val="0.156474222656474"/>
           <c:y val="0.0487799425168129"/>
-          <c:w val="0.729268909278372"/>
+          <c:w val="0.822334616932008"/>
           <c:h val="0.688243137365481"/>
         </c:manualLayout>
       </c:layout>
@@ -1081,11 +1084,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-50"/>
-        <c:axId val="-2086781888"/>
-        <c:axId val="-2118419872"/>
+        <c:axId val="2146647216"/>
+        <c:axId val="2110360864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2086781888"/>
+        <c:axId val="2146647216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1159,7 +1162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118419872"/>
+        <c:crossAx val="2110360864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1167,7 +1170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2118419872"/>
+        <c:axId val="2110360864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350.0"/>
@@ -1256,7 +1259,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086781888"/>
+        <c:crossAx val="2146647216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1291,9 +1294,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.399529688159492"/>
-          <c:y val="0.0716223592276225"/>
-          <c:w val="0.537276189716881"/>
+          <c:x val="0.492595407782056"/>
+          <c:y val="0.0204635312078922"/>
+          <c:w val="0.483444091614461"/>
           <c:h val="0.126939352619272"/>
         </c:manualLayout>
       </c:layout>
@@ -1402,8 +1405,8 @@
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>370114</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>24630</xdr:rowOff>
     </xdr:to>
@@ -1431,12 +1434,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.28748</cdr:x>
-      <cdr:y>0.05627</cdr:y>
+      <cdr:x>0.20354</cdr:x>
+      <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.39306</cdr:x>
-      <cdr:y>0.1458</cdr:y>
+      <cdr:x>0.30912</cdr:x>
+      <cdr:y>0.08953</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1445,8 +1448,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2870200" y="279400"/>
-          <a:ext cx="1054100" cy="444500"/>
+          <a:off x="2833092" y="0"/>
+          <a:ext cx="1469589" cy="444510"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1470,12 +1473,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.44776</cdr:x>
-      <cdr:y>0.27114</cdr:y>
+      <cdr:x>0.47787</cdr:x>
+      <cdr:y>0.27626</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.56224</cdr:x>
-      <cdr:y>0.36067</cdr:y>
+      <cdr:x>0.59235</cdr:x>
+      <cdr:y>0.36579</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1484,8 +1487,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4470400" y="1346200"/>
-          <a:ext cx="1143000" cy="444500"/>
+          <a:off x="6651561" y="1371591"/>
+          <a:ext cx="1593470" cy="444510"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1573,12 +1576,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.33073</cdr:x>
-      <cdr:y>0.16115</cdr:y>
+      <cdr:x>0.33894</cdr:x>
+      <cdr:y>0.16371</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.4414</cdr:x>
-      <cdr:y>0.25068</cdr:y>
+      <cdr:x>0.44961</cdr:x>
+      <cdr:y>0.25324</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1587,8 +1590,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3302000" y="800100"/>
-          <a:ext cx="1104900" cy="444500"/>
+          <a:off x="4717797" y="812798"/>
+          <a:ext cx="1540438" cy="444511"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1676,11 +1679,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.57369</cdr:x>
+      <cdr:x>0.61749</cdr:x>
       <cdr:y>0.32742</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.68817</cdr:x>
+      <cdr:x>0.73197</cdr:x>
       <cdr:y>0.41694</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -1690,8 +1693,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5727700" y="1625600"/>
-          <a:ext cx="1143000" cy="444500"/>
+          <a:off x="8594906" y="1625617"/>
+          <a:ext cx="1593470" cy="444461"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1779,11 +1782,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.69199</cdr:x>
+      <cdr:x>0.75312</cdr:x>
       <cdr:y>0.37602</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.80647</cdr:x>
+      <cdr:x>0.8676</cdr:x>
       <cdr:y>0.46555</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -1793,8 +1796,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="6908800" y="1866900"/>
-          <a:ext cx="1143000" cy="444500"/>
+          <a:off x="10482847" y="1866913"/>
+          <a:ext cx="1593470" cy="444510"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1882,12 +1885,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.81156</cdr:x>
-      <cdr:y>0.41694</cdr:y>
+      <cdr:x>0.87999</cdr:x>
+      <cdr:y>0.41182</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.92604</cdr:x>
-      <cdr:y>0.50647</cdr:y>
+      <cdr:x>0.99447</cdr:x>
+      <cdr:y>0.50135</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1896,8 +1899,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8102600" y="2070100"/>
-          <a:ext cx="1143000" cy="444500"/>
+          <a:off x="12248766" y="2044678"/>
+          <a:ext cx="1593470" cy="444510"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>

</xml_diff>